<commit_message>
Finished with WR, RB, and TE prospect models
</commit_message>
<xml_diff>
--- a/Data/wide_receiver_data_cols.xlsx
+++ b/Data/wide_receiver_data_cols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ronakmodi/FF_ProspectModel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD6D54-2EE5-924F-846E-2A46604EDB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7DBFF-2F9E-384A-A587-8D965406AC50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13260" xr2:uid="{B10F9A1B-79CC-8A4C-B620-EE4D2C8D6AB1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>hit</t>
+  </si>
+  <si>
+    <t>hit_within3years</t>
   </si>
 </sst>
 </file>
@@ -724,15 +727,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE329D8C-1103-EF4E-8083-CD8BCFD11B64}">
-  <dimension ref="A1:GV1"/>
+  <dimension ref="A1:GW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FS1" workbookViewId="0">
-      <selection activeCell="FW2" sqref="FW2"/>
+    <sheetView tabSelected="1" topLeftCell="FQ1" workbookViewId="0">
+      <selection activeCell="FW3" sqref="FW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:204" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:205" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,78 +1274,81 @@
         <v>107</v>
       </c>
       <c r="FX1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="FY1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="FY1" s="1" t="s">
+      <c r="FZ1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="FZ1" s="1" t="s">
+      <c r="GA1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GB1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="GB1" s="1" t="s">
+      <c r="GC1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="GC1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="GD1" s="1" t="s">
+      <c r="GE1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="GE1" s="1" t="s">
+      <c r="GF1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="GF1" s="1" t="s">
+      <c r="GG1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="GG1" s="1" t="s">
+      <c r="GH1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="GH1" s="1" t="s">
+      <c r="GI1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="GI1" s="1" t="s">
+      <c r="GJ1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="GJ1" s="1" t="s">
+      <c r="GK1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="GK1" s="1" t="s">
+      <c r="GL1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="GL1" s="1" t="s">
+      <c r="GM1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="GM1" s="1" t="s">
+      <c r="GN1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="GN1" s="1" t="s">
+      <c r="GO1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="GO1" s="1" t="s">
+      <c r="GP1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="GP1" s="1" t="s">
+      <c r="GQ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="GQ1" s="1" t="s">
+      <c r="GR1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="GR1" s="1" t="s">
+      <c r="GS1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="GS1" s="1" t="s">
+      <c r="GT1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="GT1" s="1" t="s">
+      <c r="GU1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="GU1" s="1" t="s">
+      <c r="GV1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="GV1" s="1" t="s">
+      <c r="GW1" s="1" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>